<commit_message>
Added some preliminary relationships
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7655AA32-0936-4B5E-A569-DB25672F657C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DCC10D-7C0B-4C21-A9E4-59C79CA3C461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
   <si>
     <t>Bob</t>
   </si>
@@ -72,13 +72,58 @@
   </si>
   <si>
     <t>vvv's opinion of &gt;&gt;&gt;</t>
+  </si>
+  <si>
+    <t>Dislikes at first but grows to [ETC]</t>
+  </si>
+  <si>
+    <t>Doesn't want to judge a book by it's cover, but is terrified once let in.</t>
+  </si>
+  <si>
+    <t>Doesn't want to let in a massive, scratching shape. Will be hostile towards it if let in.</t>
+  </si>
+  <si>
+    <t>Untrusting. Finds them suspicious.</t>
+  </si>
+  <si>
+    <t>Amicable. Finds his mission noble.</t>
+  </si>
+  <si>
+    <t>Kidnap.</t>
+  </si>
+  <si>
+    <t>Kill.</t>
+  </si>
+  <si>
+    <t>Kill. See disability as a hassle to deal with.</t>
+  </si>
+  <si>
+    <t>Kill. See fighting-age male as hostile.</t>
+  </si>
+  <si>
+    <t>Sees as being friendly and dad-like.</t>
+  </si>
+  <si>
+    <t>Neutral. He's just another guy, could be helpful.</t>
+  </si>
+  <si>
+    <t>Sees as a fellow human being and a good guy. Appreciates beard.</t>
+  </si>
+  <si>
+    <t>Neutral. Wary, but leaning towards trustworthy.</t>
+  </si>
+  <si>
+    <t>Thinks she is brave going around during the conflict. A bit too free.</t>
+  </si>
+  <si>
+    <t>Thinks she is a bit bonkers and wondering if there is a hidden agenda.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +135,13 @@
       <b/>
       <sz val="16"/>
       <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,22 +185,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,7 +516,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -478,261 +527,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="5"/>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
+      <c r="B3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="3" t="s">
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="2"/>
+      <c r="K11" s="2"/>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added more relationships and moved design doc to project
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22DCC10D-7C0B-4C21-A9E4-59C79CA3C461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2043EAD9-5F66-432D-B5BE-5B66316EA50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="32">
   <si>
     <t>Bob</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>Thinks she is a bit bonkers and wondering if there is a hidden agenda.</t>
+  </si>
+  <si>
+    <t>For once does not trust someone at the door. Questions their authority but is quiet/shy/scared.</t>
+  </si>
+  <si>
+    <t>Readys for a fight. Thinks there are no possible good intentions.</t>
+  </si>
+  <si>
+    <t>Similar to Bob. Adrenaline starts pumping and she gets ready to defend.</t>
+  </si>
+  <si>
+    <t>Hateful/angry. These kinds of people woulded Sal.</t>
+  </si>
+  <si>
+    <t>Angry/nervous of harm coming to Hal. Tries to remain stoic and calm.</t>
   </si>
 </sst>
 </file>
@@ -516,7 +531,7 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +586,9 @@
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="E2" s="2"/>
       <c r="F2" s="2" t="s">
         <v>13</v>
@@ -594,7 +611,9 @@
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2" t="s">
         <v>14</v>
@@ -615,7 +634,9 @@
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="E4" s="2"/>
       <c r="F4" s="4" t="s">
         <v>10</v>
@@ -636,7 +657,9 @@
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
@@ -659,7 +682,9 @@
       <c r="C6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
Finished minor character relationships
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2043EAD9-5F66-432D-B5BE-5B66316EA50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F77E3-4069-4168-AB75-CDEB19710D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
   <si>
     <t>Bob</t>
   </si>
@@ -74,9 +74,6 @@
     <t>vvv's opinion of &gt;&gt;&gt;</t>
   </si>
   <si>
-    <t>Dislikes at first but grows to [ETC]</t>
-  </si>
-  <si>
     <t>Doesn't want to judge a book by it's cover, but is terrified once let in.</t>
   </si>
   <si>
@@ -86,9 +83,6 @@
     <t>Untrusting. Finds them suspicious.</t>
   </si>
   <si>
-    <t>Amicable. Finds his mission noble.</t>
-  </si>
-  <si>
     <t>Kidnap.</t>
   </si>
   <si>
@@ -132,6 +126,24 @@
   </si>
   <si>
     <t>Angry/nervous of harm coming to Hal. Tries to remain stoic and calm.</t>
+  </si>
+  <si>
+    <t>Trusting. Clings to him a bit, seeing her own dad in him. Makes her think about how her parents left her.</t>
+  </si>
+  <si>
+    <t>Appreciates how he looks out for his son, but distrusts how he asks for the gun.</t>
+  </si>
+  <si>
+    <t>Relatively neutral. Thinks his mission is fruitless but doesn't tell him that.</t>
+  </si>
+  <si>
+    <t>Empathizes with her struggles and loss of parents. She motivates him even further to find his son.</t>
+  </si>
+  <si>
+    <t>Doesn't talk to Bob much. Realizes that Bob is a bit distrustful and chooses to ignore him.</t>
+  </si>
+  <si>
+    <t>Neutral. Likes her resilience and hands-on nature.</t>
   </si>
 </sst>
 </file>
@@ -526,12 +538,32 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="350" row="0">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{0F1B0929-916F-4C56-BE3F-F2994F3D62EF}">
+  <we:reference id="287764d4-2b04-4234-ba21-9a7ffa053e5c" version="1.0.0.0" store="EXCatalog" storeType="EXCatalog"/>
+  <we:alternateReferences>
+    <we:reference id="WA200002503" version="1.0.0.0" store="en-CA" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,24 +613,24 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>30</v>
+      </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
-      <c r="J2" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -606,17 +638,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -632,12 +666,14 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="F4" s="4" t="s">
         <v>10</v>
       </c>
@@ -658,7 +694,7 @@
         <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>10</v>
@@ -683,7 +719,7 @@
         <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>10</v>
@@ -738,7 +774,7 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -753,9 +789,15 @@
       <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -775,19 +817,19 @@
         <v>10</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -799,10 +841,10 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>10</v>
@@ -813,9 +855,15 @@
       <c r="H10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
+      <c r="I10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -843,8 +891,12 @@
       <c r="I11" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
+      <c r="J11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added detailed section of relationship table
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E8F77E3-4069-4168-AB75-CDEB19710D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C31D55A-9634-4A67-A886-0259F62CC283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="55">
   <si>
     <t>Bob</t>
   </si>
@@ -144,13 +144,70 @@
   </si>
   <si>
     <t>Neutral. Likes her resilience and hands-on nature.</t>
+  </si>
+  <si>
+    <t>Bob (door)</t>
+  </si>
+  <si>
+    <t>Violet (door)</t>
+  </si>
+  <si>
+    <t>Hal (door)</t>
+  </si>
+  <si>
+    <t>Sal (door)</t>
+  </si>
+  <si>
+    <t>Jessica (initial)</t>
+  </si>
+  <si>
+    <t>Bob (initial)</t>
+  </si>
+  <si>
+    <t>Violet (initial)</t>
+  </si>
+  <si>
+    <t>Hal (initial)</t>
+  </si>
+  <si>
+    <t>Sal (initial)</t>
+  </si>
+  <si>
+    <t>Jessica (over time)</t>
+  </si>
+  <si>
+    <t>Bob (over time)</t>
+  </si>
+  <si>
+    <t>Violet (over time)</t>
+  </si>
+  <si>
+    <t>Hal (over time)</t>
+  </si>
+  <si>
+    <t>Sal (over time)</t>
+  </si>
+  <si>
+    <t>See Right</t>
+  </si>
+  <si>
+    <t>Dad (door)</t>
+  </si>
+  <si>
+    <t>Dad (initial)</t>
+  </si>
+  <si>
+    <t>Dad (over time)</t>
+  </si>
+  <si>
+    <t>Detailed Table &gt;&gt;&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,8 +230,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="7" tint="0.59999389629810485"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -199,6 +279,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -212,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,6 +310,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -560,10 +670,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:AD17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,9 +681,13 @@
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="16" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" customWidth="1"/>
+    <col min="13" max="13" width="26.7109375" customWidth="1"/>
+    <col min="14" max="27" width="24.85546875" customWidth="1"/>
+    <col min="28" max="33" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -587,10 +701,10 @@
         <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -607,8 +721,65 @@
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="L1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="P1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="R1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="T1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="V1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="AC1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" s="8" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -622,18 +793,46 @@
         <v>25</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K2" s="3"/>
+      <c r="M2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="3"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+      <c r="AA2" s="7"/>
+      <c r="AB2" s="7"/>
     </row>
-    <row r="3" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -647,18 +846,46 @@
         <v>26</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="6"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="2"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
     </row>
-    <row r="4" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -671,19 +898,49 @@
       <c r="D4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="3"/>
+      <c r="J4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
+      <c r="AB4" s="7"/>
     </row>
-    <row r="5" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -699,16 +956,66 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="2"/>
+      <c r="F5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>50</v>
+      </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="I5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O5" s="6"/>
+      <c r="P5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="R5" s="12"/>
+      <c r="S5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="U5" s="12"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -724,57 +1031,129 @@
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>10</v>
+      <c r="F6" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="H6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AC6" s="7"/>
+      <c r="AD6" s="7"/>
     </row>
-    <row r="7" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="W7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="X7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Y7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+    </row>
+    <row r="8" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="B8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>10</v>
@@ -789,17 +1168,17 @@
       <c r="H8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>33</v>
+      <c r="I8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -832,7 +1211,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -865,7 +1244,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:30" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -898,11 +1277,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="17" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
All door relationships finished
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0483812-9F85-49A8-ACD0-59AA1545752F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4975210F-8F93-495E-8D0B-BA1EBA965679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
   <si>
     <t>Bob</t>
   </si>
@@ -216,6 +216,18 @@
   </si>
   <si>
     <t>Neutral. Believes that he wouldn't make an impact on food if he just stayed the night.</t>
+  </si>
+  <si>
+    <t>Takes muscular and silent nature as a trheat.</t>
+  </si>
+  <si>
+    <t>Wants to let in if Bob isn't present, otherwise will want to only let them crash for the night.</t>
+  </si>
+  <si>
+    <t>If Jessica is present he will have the same opinions. Otherwise, he will be against letting them in - too many mouths to feed.</t>
+  </si>
+  <si>
+    <t>Violet will be in favour if they have the car - more skilled members to join the party. Otherwise will have similar opinion to Bob.</t>
   </si>
 </sst>
 </file>
@@ -684,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA4" sqref="AA4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -850,12 +862,12 @@
         <v>56</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="7"/>
       <c r="AA2" s="7"/>
       <c r="AB2" s="7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>1</v>
@@ -901,7 +913,9 @@
       <c r="P3" s="9"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
-      <c r="S3" s="7"/>
+      <c r="S3" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
       <c r="V3" s="7" t="s">
@@ -913,10 +927,14 @@
       <c r="X3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="7"/>
+      <c r="Y3" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="Z3" s="7"/>
       <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
+      <c r="AB3" s="7" t="s">
+        <v>62</v>
+      </c>
       <c r="AE3" s="1" t="s">
         <v>0</v>
       </c>
@@ -975,10 +993,14 @@
       <c r="X4" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="7"/>
+      <c r="Y4" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
+      <c r="AB4" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="AE4" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
More detail on Hal and Sal, more relationships
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4975210F-8F93-495E-8D0B-BA1EBA965679}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCFA8264-9A94-4206-9AB4-E5650B2A3B6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="67">
   <si>
     <t>Bob</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>Violet will be in favour if they have the car - more skilled members to join the party. Otherwise will have similar opinion to Bob.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wants to let everyone in so encourages you to.   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutral, starts to dislike after seeing that he doesn't want to let people in </t>
   </si>
 </sst>
 </file>
@@ -342,7 +351,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -696,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -843,9 +852,11 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q2" s="7"/>
+        <v>64</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>66</v>
+      </c>
       <c r="R2" s="7"/>
       <c r="S2" s="7" t="s">
         <v>57</v>
@@ -983,7 +994,9 @@
       <c r="R4" s="7"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
+      <c r="U4" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="V4" s="7" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Work on Bob's relationships
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614AC808-D45E-4292-A03A-7A8DD2C1D977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E888F36-E20E-4874-ACA1-A8350E7FF9BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="82">
   <si>
     <t>Bob</t>
   </si>
@@ -218,9 +218,6 @@
     <t>Neutral. Believes that he wouldn't make an impact on food if he just stayed the night.</t>
   </si>
   <si>
-    <t>Takes muscular and silent nature as a trheat.</t>
-  </si>
-  <si>
     <t>Wants to let in if Bob isn't present, otherwise will want to only let them crash for the night.</t>
   </si>
   <si>
@@ -261,6 +258,30 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>Doesn't like her too much. Thinks that her trust in people is misplaced and will lead them to danger. Does appreciate her wanting to let him in.</t>
+  </si>
+  <si>
+    <t>Starts to dislike her more, but gets to know her better. She starts to change his outlook on people, showing him that growing up with a stable family can lead people in a much different direction.</t>
+  </si>
+  <si>
+    <t>Takes muscular and silent nature as a threat.</t>
+  </si>
+  <si>
+    <t>Neutral and a bit taken aback. Feels a bit bad about distrusting her but knows it's the only way to stay alive. Thinks that she will be a valuable person to have around.</t>
+  </si>
+  <si>
+    <t>Neutral. EXPAND</t>
+  </si>
+  <si>
+    <t>Comes to appreciate her more. Admires her fearlessness and resolution, and finds her skills very helpful.</t>
+  </si>
+  <si>
+    <t>Pities her - another kid with a rough family situation forced out into hostile conditions. Appreciates the task she's taken upon herself to protect and help her brother. Does find her optimism as a downside.</t>
+  </si>
+  <si>
+    <t>Pities him but likes that he was injured protecting his sister and fighting for his freedom. Thinks that having a casualty could hinder the party, but knows the skills would be valuable.</t>
   </si>
 </sst>
 </file>
@@ -729,8 +750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,22 +897,22 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
       <c r="P2" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S2" s="7" t="s">
         <v>57</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="V2" s="7" t="s">
         <v>57</v>
@@ -903,22 +924,22 @@
         <v>56</v>
       </c>
       <c r="Y2" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Z2" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA2" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AB2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="AB2" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC2" s="7" t="s">
-        <v>72</v>
-      </c>
       <c r="AD2" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AE2" s="1" t="s">
         <v>1</v>
@@ -959,16 +980,24 @@
       <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
+      <c r="N3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>75</v>
+      </c>
       <c r="P3" s="9"/>
       <c r="Q3" s="10"/>
       <c r="R3" s="10"/>
       <c r="S3" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
+        <v>76</v>
+      </c>
+      <c r="T3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="U3" s="7" t="s">
+        <v>79</v>
+      </c>
       <c r="V3" s="7" t="s">
         <v>58</v>
       </c>
@@ -979,14 +1008,18 @@
         <v>55</v>
       </c>
       <c r="Y3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z3" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="Z3" s="7" t="s">
+        <v>80</v>
+      </c>
       <c r="AA3" s="7"/>
       <c r="AB3" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC3" s="7"/>
+        <v>61</v>
+      </c>
+      <c r="AC3" s="7" t="s">
+        <v>81</v>
+      </c>
       <c r="AD3" s="7"/>
       <c r="AE3" s="1" t="s">
         <v>0</v>
@@ -1027,17 +1060,19 @@
       <c r="M4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
       <c r="P4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="7"/>
+      <c r="Q4" s="7" t="s">
+        <v>78</v>
+      </c>
       <c r="R4" s="7"/>
       <c r="S4" s="10"/>
       <c r="T4" s="10"/>
       <c r="U4" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="V4" s="7" t="s">
         <v>59</v>
@@ -1049,12 +1084,12 @@
         <v>56</v>
       </c>
       <c r="Y4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Z4" s="7"/>
       <c r="AA4" s="7"/>
       <c r="AB4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AC4" s="7"/>
       <c r="AD4" s="7"/>
@@ -1097,7 +1132,7 @@
       <c r="M5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="7" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="4" t="s">
@@ -1209,10 +1244,10 @@
         <v>10</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AD6" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AE6" s="1" t="s">
         <v>3</v>
@@ -1278,10 +1313,10 @@
         <v>10</v>
       </c>
       <c r="Z7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AA7" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>

</xml_diff>

<commit_message>
Finished Hal and Sal relationships
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ED5DA59-FC63-47E5-B4B2-48667D7080FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED377F88-6F28-4B59-A6CA-CCAC4EFEFF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="92">
   <si>
     <t>Bob</t>
   </si>
@@ -269,9 +269,6 @@
     <t>Pities him but likes that he was injured protecting his sister and fighting for his freedom. Thinks that having a casualty could hinder the party, but knows the skills would be valuable.</t>
   </si>
   <si>
-    <t>Enjoys some younger company and appreciates Hal's positive outlook on the situation. Does find that he talks a bit too much and asks too many questions.</t>
-  </si>
-  <si>
     <t>Staert to become friends quickly. Relates with Jessica's disability. Isn't too fond of her snooty rich upbringing but knows it wasn't her fault.</t>
   </si>
   <si>
@@ -291,6 +288,30 @@
   </si>
   <si>
     <t>Neutral. Doesn't really "talk" to Sal, and he's both quiet and sick to begin with.</t>
+  </si>
+  <si>
+    <t>Doesn't voice it, but believes that she will hinder the party (even being injured himself). Finds that she brings nothing, consumes food, and holds back the party with her disability.</t>
+  </si>
+  <si>
+    <t>Silently appreciates him. Relates to him in many ways, even with their situations being vastly different. Feels a bit "inspired" to be like him - resourceful, cunning, calculated.</t>
+  </si>
+  <si>
+    <t>Likes her. Gets a bit frustrated trying to communicate, especially being ill. Thinks that she will be helpful in getting them where they need to go.</t>
+  </si>
+  <si>
+    <t>Feels a bit bad for her being disabled and treats her like a bit of an aunt. Will gladly yap</t>
+  </si>
+  <si>
+    <t>Enjoys some younger company and appreciates Hal's positive outlook on the situation. Does find that she talks a bit too much and asks too many questions.</t>
+  </si>
+  <si>
+    <t>Feels a bit bad for her being disabled and treats her like a bit of an aunt. Will gladly yap on and on without realizing that Jessica doesn't care and is getting a bit fed up.</t>
+  </si>
+  <si>
+    <t>Finds him to be a bit grumpy. Feels like he sees the worst in people when things really aren't all that bad. Thinks that he'll come around eventually.</t>
+  </si>
+  <si>
+    <t>Feels like they have good energy going. Imagines them tag-teaming problems, Violet the brawn and her the brain. Doesn't actually talk to her that much.</t>
   </si>
 </sst>
 </file>
@@ -388,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,9 +425,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -759,8 +777,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,55 +833,55 @@
       <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="O1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="R1" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="S1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="W1" s="8" t="s">
+      <c r="W1" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="X1" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AC1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AD1" s="7" t="s">
         <v>47</v>
       </c>
       <c r="AE1" s="1"/>
@@ -884,67 +902,67 @@
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J2" s="11" t="s">
+      <c r="F2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J2" s="10" t="s">
         <v>53</v>
       </c>
       <c r="K2" s="3"/>
       <c r="M2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="7" t="s">
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="Q2" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="S2" s="7" t="s">
+      <c r="S2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="T2" s="7" t="s">
+      <c r="T2" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="U2" s="7" t="s">
+      <c r="U2" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="V2" s="7" t="s">
+      <c r="V2" s="6" t="s">
         <v>57</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="7" t="s">
+      <c r="X2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Y2" s="7" t="s">
+      <c r="Y2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="Z2" s="7" t="s">
-        <v>77</v>
+      <c r="Z2" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="7" t="s">
+      <c r="AB2" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="6" t="s">
         <v>68</v>
       </c>
       <c r="AD2" s="4" t="s">
@@ -970,65 +988,65 @@
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I3" s="11" t="s">
+      <c r="F3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="J3" s="3"/>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="M3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="N3" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="P3" s="9"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="7" t="s">
+      <c r="P3" s="8"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="6" t="s">
         <v>58</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="X3" s="7" t="s">
+      <c r="X3" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="Y3" s="7" t="s">
+      <c r="Y3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="Z3" s="7" t="s">
+      <c r="Z3" s="6" t="s">
         <v>75</v>
       </c>
       <c r="AA3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AB3" s="7" t="s">
+      <c r="AB3" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AC3" s="6" t="s">
         <v>76</v>
       </c>
       <c r="AD3" s="4" t="s">
@@ -1054,68 +1072,68 @@
       <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H4" s="11" t="s">
+      <c r="F4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>53</v>
       </c>
       <c r="I4" s="3"/>
-      <c r="J4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K4" s="11" t="s">
+      <c r="J4" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K4" s="10" t="s">
         <v>53</v>
       </c>
       <c r="M4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="N4" s="7" t="s">
+      <c r="N4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="O4" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q4" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="P4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V4" s="7" t="s">
-        <v>82</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="X4" s="7" t="s">
+      <c r="X4" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="Y4" s="7" t="s">
+      <c r="Y4" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="Z4" s="7" t="s">
+      <c r="Z4" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="AC4" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB4" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="AC4" s="7" t="s">
-        <v>84</v>
       </c>
       <c r="AD4" s="4" t="s">
         <v>10</v>
@@ -1140,26 +1158,26 @@
       <c r="E5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="11" t="s">
+      <c r="F5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="11" t="s">
+      <c r="I5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>53</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="7" t="s">
+      <c r="N5" s="6" t="s">
         <v>32</v>
       </c>
       <c r="O5" s="4" t="s">
@@ -1183,9 +1201,9 @@
       <c r="U5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="9"/>
+      <c r="X5" s="9"/>
       <c r="Y5" s="4" t="s">
         <v>10</v>
       </c>
@@ -1224,37 +1242,49 @@
       <c r="E6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="10" t="s">
         <v>53</v>
       </c>
       <c r="G6" s="3"/>
-      <c r="H6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="11" t="s">
+      <c r="H6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" s="10" t="s">
         <v>53</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="N6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
+      <c r="Q6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="S6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
+      <c r="T6" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="U6" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="V6" s="4" t="s">
         <v>10</v>
       </c>
@@ -1264,16 +1294,16 @@
       <c r="X6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Y6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
       <c r="AB6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AC6" s="7" t="s">
+      <c r="AC6" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AD6" s="7" t="s">
+      <c r="AD6" s="6" t="s">
         <v>65</v>
       </c>
       <c r="AE6" s="1" t="s">
@@ -1297,36 +1327,48 @@
         <v>10</v>
       </c>
       <c r="F7" s="3"/>
-      <c r="G7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="11" t="s">
+      <c r="G7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="10" t="s">
         <v>53</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
+      <c r="N7" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="P7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
+      <c r="Q7" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="S7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
+      <c r="T7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" s="4" t="s">
+        <v>10</v>
+      </c>
       <c r="V7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1339,15 +1381,15 @@
       <c r="Y7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="Z7" s="7" t="s">
+      <c r="Z7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AA7" s="7" t="s">
+      <c r="AA7" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="AB7" s="10"/>
-      <c r="AC7" s="10"/>
-      <c r="AD7" s="10"/>
+      <c r="AB7" s="9"/>
+      <c r="AC7" s="9"/>
+      <c r="AD7" s="9"/>
       <c r="AE7" s="1" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Tweaked one sibling line
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED377F88-6F28-4B59-A6CA-CCAC4EFEFF04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5C1F01-3865-49E2-82E2-617790760F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -778,7 +778,7 @@
   <dimension ref="A1:AE17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Day 6 night complete
</commit_message>
<xml_diff>
--- a/Relationships.xlsx
+++ b/Relationships.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Tech\Unity Projects\BeyondTheDoor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB5C1F01-3865-49E2-82E2-617790760F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{101EA3B0-7380-487F-AF1B-CF2B0B206CDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{CDC396D3-33B3-43AC-B8AC-AB6F001B02AB}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="91">
   <si>
     <t>Bob</t>
   </si>
@@ -297,9 +297,6 @@
   </si>
   <si>
     <t>Likes her. Gets a bit frustrated trying to communicate, especially being ill. Thinks that she will be helpful in getting them where they need to go.</t>
-  </si>
-  <si>
-    <t>Feels a bit bad for her being disabled and treats her like a bit of an aunt. Will gladly yap</t>
   </si>
   <si>
     <t>Enjoys some younger company and appreciates Hal's positive outlook on the situation. Does find that she talks a bit too much and asks too many questions.</t>
@@ -459,9 +456,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -499,7 +496,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -605,7 +602,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -747,7 +744,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -777,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DC22092-451E-4600-BA90-9AA6F087C231}">
   <dimension ref="A1:AE17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="T1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +951,7 @@
         <v>59</v>
       </c>
       <c r="Z2" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AA2" s="4" t="s">
         <v>10</v>
@@ -1262,25 +1259,25 @@
         <v>3</v>
       </c>
       <c r="N6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="O6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="R6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>90</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>91</v>
       </c>
       <c r="U6" s="4" t="s">
         <v>10</v>

</xml_diff>